<commit_message>
Kevin: Accidentally fixed a bug while trying to fix another bug
</commit_message>
<xml_diff>
--- a/output/OPEN/JTC000ETT22000053/JTC000ETT22000053.xlsx
+++ b/output/OPEN/JTC000ETT22000053/JTC000ETT22000053.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>Contact Person's Address</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>29 Apr 2022 04:00PM</t>
@@ -98,6 +95,12 @@
 3) FULLY ELECTRONIC SUBMISSION (2-ENVELOPES Price-Quality Method): Contractor are required to submit their "PRICE" and "QUALITY" proposals electronically via GeBiz. The Form of Tender, Breakdown Costs of Tender and Final Summary and Life-cycle cost must be submitted into GeBiz's "PRICE" Envelope while Quality proposal must be submitted into GeBIZ"s "QUALITY" Envelope.
 4) Tenderer must be registered with BCA under the work head ME-04_ with the financial grade of L6 (unlimited)
 Eligibility Criteria: Tenderers are advised to refer to the Critical Criteria under the Tender Evaluation section of the Invitation of Tender, to check on your tendering eligibility before they prepare your Tender Proposal.</t>
+  </si>
+  <si>
+    <t>Daniel_CHEONG@jtc.gov.sg</t>
+  </si>
+  <si>
+    <t>The JTC Summit, 8 Jurong Town Hall Road, Singapore 609434</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -483,7 +486,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="216" x14ac:dyDescent="0.3">
@@ -491,7 +494,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -507,31 +510,28 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
-        <v>19</v>
+      <c r="B11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>